<commit_message>
semenov et al 2007 and tidying up metadata extraction file
</commit_message>
<xml_diff>
--- a/thesis metadata.xlsx
+++ b/thesis metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8212092E-8657-CC43-A262-E7C8505DBAD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DEDC00-97BF-2A4A-84A2-4BE58714E679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-1220" windowWidth="24000" windowHeight="11160" xr2:uid="{10A247D6-D658-0F47-8BA3-8B88B4069902}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{F38E8EE3-8927-4E47-8FE4-3E7F9175C870}">
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{F38E8EE3-8927-4E47-8FE4-3E7F9175C870}">
       <text>
         <r>
           <rPr>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
   <si>
     <t xml:space="preserve">decoding </t>
   </si>
@@ -163,21 +163,9 @@
     <t>species richness, ecosystem?</t>
   </si>
   <si>
-    <t>min_time</t>
-  </si>
-  <si>
-    <t>max_time</t>
-  </si>
-  <si>
     <t>pre-experimental temperature</t>
   </si>
   <si>
-    <t xml:space="preserve">amount of time in hours spent at minimum temperature </t>
-  </si>
-  <si>
-    <t xml:space="preserve">amount of time in hours spent at maximum temperature </t>
-  </si>
-  <si>
     <t xml:space="preserve">definition of experimental result </t>
   </si>
   <si>
@@ -269,6 +257,15 @@
   </si>
   <si>
     <t xml:space="preserve">plant, animal, fungi, bacteria </t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">very small, small, medium, large </t>
+  </si>
+  <si>
+    <t>period_flux</t>
   </si>
 </sst>
 </file>
@@ -635,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8067244D-934C-9B4E-868B-490E47214A9B}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,10 +654,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -668,7 +665,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -701,16 +698,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -718,7 +715,7 @@
         <v>8</v>
       </c>
       <c r="J7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -738,118 +735,118 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" t="s">
         <v>32</v>
-      </c>
-      <c r="J12" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
+        <v>11</v>
+      </c>
+      <c r="J16" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
       </c>
       <c r="J17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="J18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
       </c>
       <c r="J21" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
-      </c>
-      <c r="J22" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -857,7 +854,7 @@
         <v>7</v>
       </c>
       <c r="J24" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -870,21 +867,21 @@
         <v>23</v>
       </c>
       <c r="J26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -902,18 +899,18 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J30" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J31" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>